<commit_message>
add corrected input files
</commit_message>
<xml_diff>
--- a/data/Fall2018/db1-7_all-timepoints-runs/db2/14-gene_25-edges_db2_Sigmoid_estimation_all-timepoints.xlsx
+++ b/data/Fall2018/db1-7_all-timepoints-runs/db2/14-gene_25-edges_db2_Sigmoid_estimation_all-timepoints.xlsx
@@ -859,7 +859,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -871,7 +871,7 @@
     <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -879,7 +879,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -887,7 +887,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -895,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -903,7 +903,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -911,7 +911,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -919,7 +919,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -927,7 +927,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -935,7 +935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -988,8 +988,14 @@
       <c r="D14" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E14" s="3">
+        <v>90</v>
+      </c>
+      <c r="F14" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1051,6 +1057,42 @@
       </c>
       <c r="N16" s="3">
         <v>60</v>
+      </c>
+      <c r="O16" s="3">
+        <v>65</v>
+      </c>
+      <c r="P16" s="3">
+        <v>70</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>75</v>
+      </c>
+      <c r="R16" s="3">
+        <v>80</v>
+      </c>
+      <c r="S16" s="3">
+        <v>85</v>
+      </c>
+      <c r="T16" s="3">
+        <v>90</v>
+      </c>
+      <c r="U16" s="3">
+        <v>95</v>
+      </c>
+      <c r="V16" s="3">
+        <v>100</v>
+      </c>
+      <c r="W16" s="3">
+        <v>105</v>
+      </c>
+      <c r="X16" s="3">
+        <v>110</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>115</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>